<commit_message>
History Chapter 2 completed
</commit_message>
<xml_diff>
--- a/daily routine.xlsx
+++ b/daily routine.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>current affairs</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Chapter 1--&gt;5th- 10th</t>
   </si>
   <si>
-    <t xml:space="preserve">chapter 2--&gt;6th - 9th </t>
-  </si>
-  <si>
     <t>Chapter 2 --&gt; 5th-7th</t>
   </si>
   <si>
@@ -121,6 +118,12 @@
   </si>
   <si>
     <t>office work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chapter 2--&gt;6th - 10th </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chapter 3--&gt;11th - 13th </t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -651,7 +654,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>3</v>
@@ -698,23 +701,23 @@
         <v>13</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -723,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>8</v>
@@ -732,10 +735,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="J3" s="3"/>
       <c r="L3" s="3"/>
@@ -745,7 +748,7 @@
     <row r="4" spans="1:14" ht="30">
       <c r="A4" s="5"/>
       <c r="B4" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
@@ -762,7 +765,7 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -773,20 +776,20 @@
     <row r="5" spans="1:14" ht="30">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="22"/>
       <c r="F5" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -794,14 +797,16 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" ht="30">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D6" s="12"/>
       <c r="E6" s="23"/>
       <c r="F6" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>

</xml_diff>

<commit_message>
Economics(Chapter 3) & Geography(Chapter 2) completed
</commit_message>
<xml_diff>
--- a/daily routine.xlsx
+++ b/daily routine.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>current affairs</t>
   </si>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">Chapter 1--&gt;4th </t>
   </si>
   <si>
-    <t>Chapter 1--&gt;5th- 10th</t>
-  </si>
-  <si>
     <t>Chapter 2 --&gt; 5th-7th</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>https://unacademy.com/lesson/3rd-april-2017-daily-mcqs-on-current-affairs-for-government-exams-upsc-cseias-exam/CPZHFQM3</t>
   </si>
   <si>
-    <t>Chapter 3--&gt;8th-10th</t>
-  </si>
-  <si>
     <t>office work</t>
   </si>
   <si>
@@ -124,6 +118,21 @@
   </si>
   <si>
     <t xml:space="preserve">chapter 3--&gt;11th - 13th </t>
+  </si>
+  <si>
+    <t>Chapter 2--&gt;9th</t>
+  </si>
+  <si>
+    <t>Chapter 3--&gt;10th-11th</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>Chapter 1</t>
+  </si>
+  <si>
+    <t>Chapter 3--&gt;9th-10th</t>
   </si>
 </sst>
 </file>
@@ -166,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +206,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -284,6 +305,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -292,7 +324,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,7 +343,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,12 +360,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -632,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -646,15 +695,15 @@
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="12" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>3</v>
@@ -665,7 +714,7 @@
       <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="9" t="s">
@@ -674,15 +723,14 @@
       <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="23"/>
       <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -690,593 +738,464 @@
       <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="L2" s="23"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="23"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="30">
+    </row>
+    <row r="4" spans="1:13" ht="30">
       <c r="A4" s="5"/>
-      <c r="B4" s="10" t="s">
-        <v>30</v>
+      <c r="B4" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="23"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="30">
+      <c r="A5" s="3"/>
+      <c r="B5" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="30">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="17" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="H5" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="23"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="30">
+    </row>
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="23"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="I7" s="26"/>
+      <c r="L7" s="23"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="I8" s="26"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14">
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="I9" s="26"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="I10" s="26"/>
+      <c r="L10" s="23"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="I11" s="26"/>
+      <c r="L11" s="23"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="I12" s="26"/>
+      <c r="L12" s="23"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="G13" s="5"/>
+      <c r="I13" s="26"/>
+      <c r="L13" s="23"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="I14" s="26"/>
+      <c r="L14" s="23"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="I15" s="26"/>
+      <c r="L15" s="23"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="I16" s="26"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14">
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="I17" s="26"/>
+      <c r="L17" s="23"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14">
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="I18" s="26"/>
+      <c r="L18" s="23"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14">
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="I19" s="26"/>
+      <c r="L19" s="23"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14">
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="I20" s="26"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14">
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="I21" s="26"/>
+      <c r="L21" s="23"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14">
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="I22" s="26"/>
+      <c r="L22" s="23"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14">
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="I23" s="26"/>
+      <c r="L23" s="23"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14">
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="I24" s="26"/>
+      <c r="L24" s="23"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14">
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="I25" s="26"/>
+      <c r="L25" s="23"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14">
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="I26" s="26"/>
+      <c r="L26" s="23"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14">
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="I27" s="26"/>
+      <c r="L27" s="23"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:14">
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="I28" s="26"/>
+      <c r="L28" s="23"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14">
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="I29" s="26"/>
+      <c r="L29" s="23"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:14">
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="I30" s="26"/>
+      <c r="L30" s="23"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14">
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="I31" s="26"/>
+      <c r="L31" s="23"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:14">
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="I32" s="26"/>
+      <c r="L32" s="23"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="1:14">
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="I33" s="26"/>
+      <c r="L33" s="23"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14">
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+      <c r="I34" s="26"/>
+      <c r="L34" s="23"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14">
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="I35" s="26"/>
+      <c r="L35" s="23"/>
       <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14">
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="I36" s="26"/>
+      <c r="L36" s="23"/>
       <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E6"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>